<commit_message>
Fixing the Plots for Exercise week 2
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Codebook" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>